<commit_message>
tambah listener dan reporting
</commit_message>
<xml_diff>
--- a/src/test/resources/Data/LoginData.xlsx
+++ b/src/test/resources/Data/LoginData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Downloads\Project-Assigment-day-28\src\test\resources\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Berkas QA engineer\Project-Assigment-day-29\src\test\resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD0300EE-D8F9-4774-B266-354B0CAEDC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34013578-531D-497E-AEFE-AAECBED89BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>